<commit_message>
Updated files, html corresponds to blog post
</commit_message>
<xml_diff>
--- a/Moody's Chart.xlsx
+++ b/Moody's Chart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>reso</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6677,8 +6685,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="323873400"/>
-        <c:axId val="323873008"/>
+        <c:axId val="249879880"/>
+        <c:axId val="249880272"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -6800,11 +6808,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="423854208"/>
-        <c:axId val="423853032"/>
+        <c:axId val="249881056"/>
+        <c:axId val="249880664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="323873400"/>
+        <c:axId val="249879880"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -6920,12 +6928,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="323873008"/>
+        <c:crossAx val="249880272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="323873008"/>
+        <c:axId val="249880272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7038,12 +7046,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="323873400"/>
+        <c:crossAx val="249879880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="423853032"/>
+        <c:axId val="249880664"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7143,12 +7151,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="423854208"/>
+        <c:crossAx val="249881056"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="423854208"/>
+        <c:axId val="249881056"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7159,7 +7167,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="423853032"/>
+        <c:crossAx val="249880664"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -7202,7 +7211,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
   <c:userShapes r:id="rId3"/>
 </c:chartSpace>
@@ -7810,8 +7819,8 @@
       <cdr:x>0.19255</cdr:x>
       <cdr:y>0.38864</cdr:y>
     </cdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="2" name="TextBox 1"/>
@@ -7842,6 +7851,7 @@
               </a:r>
             </a:p>
             <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -7881,7 +7891,7 @@
           </cdr:txBody>
         </cdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="2" name="TextBox 1"/>
@@ -9032,7 +9042,7 @@
         <v>0.102733857706594</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16750.4027023417</v>
       </c>
@@ -9067,7 +9077,7 @@
         <v>0.102629772621134</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18554.467069652899</v>
       </c>
@@ -9101,8 +9111,11 @@
       <c r="K18">
         <v>0.10253568992987901</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20552.8341232479</v>
       </c>
@@ -9137,7 +9150,7 @@
         <v>0.10245065855826301</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>22766.430795991</v>
       </c>
@@ -9172,7 +9185,7 @@
         <v>0.102373816020919</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>25218.4379088803</v>
       </c>
@@ -9207,7 +9220,7 @@
         <v>0.10230438050484</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>27934.532920990099</v>
       </c>
@@ -9242,7 +9255,7 @@
         <v>0.102241643598884</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>30943.158824246399</v>
       </c>
@@ -9277,7 +9290,7 @@
         <v>0.102184963628245</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>34275.821998909698</v>
       </c>
@@ -9312,7 +9325,7 @@
         <v>0.102133759552913</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>37967.422148910096</v>
       </c>
@@ -9347,7 +9360,7 @@
         <v>0.102087505390056</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>42056.617772125501</v>
       </c>
@@ -9382,7 +9395,7 @@
         <v>0.10204572512163999</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>46586.230992810102</v>
       </c>
@@ -9417,7 +9430,7 @@
         <v>0.102007988050218</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>51603.695995589303</v>
       </c>
@@ -9452,7 +9465,7 @@
         <v>0.101973904567684</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>57161.555757025802</v>
       </c>
@@ -9487,7 +9500,7 @@
         <v>0.101943229521513</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>63318.012276540103</v>
       </c>
@@ -9522,7 +9535,7 @@
         <v>0.101915404425787</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>70137.536068711794</v>
       </c>
@@ -9557,7 +9570,7 @@
         <v>0.101890217440004</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>77691.541299575794</v>
       </c>

</xml_diff>